<commit_message>
Allow half days selection
Change the working days field to a decimal and change all the relevant references.  Add in a new set of calculations to the excel document to help aid testing.

Update the About page to include details on the new version changes + changes that wern't documented for the patch release in the summer.
</commit_message>
<xml_diff>
--- a/Working days calculations.xlsx
+++ b/Working days calculations.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\visualstudio\retirement-countdown-clock\trunk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\retirement-countdown-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="4695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>holidays</t>
   </si>
@@ -34,12 +34,27 @@
   <si>
     <t>working days</t>
   </si>
+  <si>
+    <t>Working Days</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Calendar days</t>
+  </si>
+  <si>
+    <t>Working days</t>
+  </si>
+  <si>
+    <t>pct</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,13 +62,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,9 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,19 +381,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>42407</v>
       </c>
@@ -377,8 +413,37 @@
         <f>E5/365.25</f>
         <v>0.80219028062970565</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+      <c r="L6">
+        <f>(K6*2)-1</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>(N6+1)/2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -389,8 +454,22 @@
         <f>ROUND(C7*F5,0)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L19" si="0">(K7*2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O18" si="1">(N7+1)/2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -401,8 +480,22 @@
         <f>ROUND(C8*F5,0)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1.5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -413,14 +506,431 @@
         <f>ROUND(C9*(E5/7),0)</f>
         <v>209</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>2.5</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E11">
         <f>E9-E8-E7</f>
         <v>184</v>
       </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>3.5</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <v>6</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <v>7</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>4.5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N14">
+        <v>8</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="N15">
+        <v>9</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>5.5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="N17">
+        <v>11</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <v>6.5</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N18">
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>3157</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f>D19/7</f>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f>ROUNDUP(C19*E19, 0)</f>
+        <v>3157</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="N19">
+        <v>13</v>
+      </c>
+      <c r="O19">
+        <f>(N19+1)/2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f>C19</f>
+        <v>3157</v>
+      </c>
+      <c r="D20">
+        <v>6.5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:E31" si="2">D20/7</f>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F20">
+        <f>ROUNDUP(C20*E20, 0)</f>
+        <v>2932</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" ref="C21:C32" si="3">C20</f>
+        <v>3157</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F32" si="4">ROUNDUP(C21*E21, 0)</f>
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D22">
+        <v>5.5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D24">
+        <v>4.5</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D26">
+        <v>3.5</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D28">
+        <v>2.5</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D30">
+        <v>1.5</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>3157</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <f>D32/7</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>226</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>